<commit_message>
trained the HDHGN on Python and C files
</commit_message>
<xml_diff>
--- a/backend/HDHGN/work_dir/results_c.xlsx
+++ b/backend/HDHGN/work_dir/results_c.xlsx
@@ -450,14 +450,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 25 </t>
+          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 26 </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.02</v>
+        <v>0.8557692307692307</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06</v>
+        <v>0.9038461538461539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added a TrainModel function in /HDHGN - trained model on the modifyied source files set
</commit_message>
<xml_diff>
--- a/backend/HDHGN/work_dir/results_c.xlsx
+++ b/backend/HDHGN/work_dir/results_c.xlsx
@@ -450,14 +450,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 26 </t>
+          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 25 </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8557692307692307</v>
+        <v>0.2</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9038461538461539</v>
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Model retrain on modyfied fiels for more prediction flexibility.
</commit_message>
<xml_diff>
--- a/backend/HDHGN/work_dir/results_c.xlsx
+++ b/backend/HDHGN/work_dir/results_c.xlsx
@@ -450,14 +450,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 25 </t>
+          <t xml:space="preserve">embed size=128 dim size=128 num layers=4 num_edge_heads=8num_node_heads=8 num_heads=8 dropout=0.2 feed size=128 1024 24 </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.2</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>